<commit_message>
fix: overall business process.
</commit_message>
<xml_diff>
--- a/src/main/resources/RewardAmountNew.xlsx
+++ b/src/main/resources/RewardAmountNew.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danil\Documents\Desarrollo\Zubale\del.kogito-example-main\kogito-example-main\src\main\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448650C9-A282-4BE3-B6B8-78918967228F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>RuleSet</t>
   </si>
@@ -19,12 +28,6 @@
     <t>com.zubale.quest</t>
   </si>
   <si>
-    <t>Unit</t>
-  </si>
-  <si>
-    <t>Quest</t>
-  </si>
-  <si>
     <t>Import</t>
   </si>
   <si>
@@ -55,12 +58,6 @@
     <t>$quest.platform == "$param"</t>
   </si>
   <si>
-    <t>$quest.distance $param</t>
-  </si>
-  <si>
-    <t>lines $param</t>
-  </si>
-  <si>
     <t>$quest.setRewardAmount(Float.parseFloat("$1"));</t>
   </si>
   <si>
@@ -79,85 +76,76 @@
     <t>petco</t>
   </si>
   <si>
-    <t>&lt; 3</t>
-  </si>
-  <si>
-    <t>&lt;= 3</t>
-  </si>
-  <si>
     <t>REWARD_AMOUNT_NEW</t>
   </si>
   <si>
     <t>walmart</t>
   </si>
   <si>
-    <t>&lt; 5</t>
-  </si>
-  <si>
-    <t>&gt; 3</t>
-  </si>
-  <si>
     <t>general</t>
   </si>
   <si>
-    <t>&gt;= 7</t>
-  </si>
-  <si>
-    <t>&lt;= 2</t>
+    <t>$quest.distance &lt; $param</t>
+  </si>
+  <si>
+    <t>$quest.lines &lt;= $param</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="8.0"/>
+      <sz val="8"/>
       <color theme="0"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="8.0"/>
+      <sz val="8"/>
       <color rgb="FFFFFFFF"/>
       <name val="Tahoma"/>
     </font>
     <font>
-      <sz val="8.0"/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="8.0"/>
+      <sz val="8"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
     </font>
-    <font/>
-    <font>
-      <sz val="8.0"/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Tahoma"/>
     </font>
     <font>
-      <sz val="8.0"/>
+      <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="8.0"/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Tahoma"/>
     </font>
     <font>
-      <sz val="8.0"/>
+      <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Docs-Tahoma"/>
     </font>
@@ -167,7 +155,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -207,41 +195,54 @@
     </fill>
   </fills>
   <borders count="5">
-    <border/>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -251,88 +252,93 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+  <cellXfs count="23">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -522,26 +528,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="23.57"/>
-    <col customWidth="1" min="2" max="2" width="41.14"/>
-    <col customWidth="1" min="3" max="3" width="28.43"/>
-    <col customWidth="1" min="4" max="5" width="35.14"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" customWidth="1"/>
+    <col min="4" max="5" width="35.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -553,201 +564,193 @@
       <c r="E1" s="3"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="4"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:7">
+      <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>5</v>
+      <c r="B3" s="7" t="b">
+        <v>1</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="F3" s="8"/>
+      <c r="F3" s="7"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:7">
+      <c r="A4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="9" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="10" t="s">
+      <c r="B7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="E7" s="10" t="s">
+        <v>9</v>
+      </c>
       <c r="F7" s="5"/>
-      <c r="G7" s="11"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="13" t="s">
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="13" t="s">
-        <v>11</v>
-      </c>
+      <c r="B8" s="19"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9">
-      <c r="A9" s="14" t="s">
+    <row r="9" spans="1:7">
+      <c r="A9" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10">
-      <c r="A10" s="16" t="s">
+    <row r="10" spans="1:7">
+      <c r="A10" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="13" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13" t="s">
+      <c r="D10" s="14"/>
+      <c r="E10" s="15" t="s">
         <v>16</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11">
-      <c r="A11" s="17" t="s">
+    <row r="11" spans="1:7">
+      <c r="A11" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="16">
+        <v>3</v>
+      </c>
+      <c r="C11" s="16">
+        <v>3</v>
+      </c>
+      <c r="D11" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="19" t="s">
-        <v>20</v>
+      <c r="E11" s="16">
+        <v>100</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12">
-      <c r="A12" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="20">
-        <v>100.0</v>
+    <row r="12" spans="1:7">
+      <c r="A12" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="16">
+        <v>5</v>
+      </c>
+      <c r="C12" s="16">
+        <v>3</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="16">
+        <v>200</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13">
-      <c r="A13" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="20">
-        <v>200.0</v>
+    <row r="13" spans="1:7">
+      <c r="A13" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="16">
+        <v>7</v>
+      </c>
+      <c r="C13" s="16">
+        <v>2</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="16">
+        <v>150</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
-    <row r="14">
-      <c r="A14" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="20">
-        <v>150.0</v>
-      </c>
-      <c r="F14" s="5"/>
+    <row r="14" spans="1:7">
       <c r="G14" s="5"/>
-    </row>
-    <row r="15">
-      <c r="G15" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B4:F4"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>